<commit_message>
Updates to the variant caller
The new code increases yields by about 15% by not discarding certain types of MNVs
</commit_message>
<xml_diff>
--- a/data/codon_table.xlsx
+++ b/data/codon_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiderinam/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/hzi14_psu_edu/Documents/RProjects/duplex_sequencing_screen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD8583E0-411A-A54E-86DB-C825A109019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CD8583E0-411A-A54E-86DB-C825A109019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{866A84EA-99AE-474F-8263-035D6DBFE9F8}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{2013C8B1-2B53-2846-AC66-2AF3C3C26FC0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="132">
   <si>
     <t>Letter</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>FullName</t>
+  </si>
+  <si>
+    <t>Twist</t>
   </si>
 </sst>
 </file>
@@ -777,13 +780,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87D0E51-E1D1-9A4C-8B73-1E92A7B80DE1}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -796,8 +799,11 @@
       <c r="D1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -810,8 +816,11 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -824,8 +833,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -838,8 +850,11 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -852,8 +867,11 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -866,8 +884,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -880,8 +901,11 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -894,8 +918,11 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -908,8 +935,11 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -922,8 +952,11 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -936,8 +969,11 @@
       <c r="D11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -950,8 +986,11 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -964,8 +1003,11 @@
       <c r="D13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -978,8 +1020,11 @@
       <c r="D14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -992,8 +1037,11 @@
       <c r="D15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1006,8 +1054,11 @@
       <c r="D16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1020,8 +1071,11 @@
       <c r="D17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1034,8 +1088,11 @@
       <c r="D18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1048,8 +1105,11 @@
       <c r="D19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1062,8 +1122,11 @@
       <c r="D20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1076,8 +1139,11 @@
       <c r="D21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1090,8 +1156,11 @@
       <c r="D22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1104,8 +1173,11 @@
       <c r="D23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1118,8 +1190,11 @@
       <c r="D24" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1132,8 +1207,11 @@
       <c r="D25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1146,8 +1224,11 @@
       <c r="D26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1160,8 +1241,11 @@
       <c r="D27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1174,8 +1258,11 @@
       <c r="D28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1188,8 +1275,11 @@
       <c r="D29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1202,8 +1292,11 @@
       <c r="D30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1216,8 +1309,11 @@
       <c r="D31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -1230,8 +1326,11 @@
       <c r="D32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1244,8 +1343,11 @@
       <c r="D33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1258,8 +1360,11 @@
       <c r="D34" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -1272,8 +1377,11 @@
       <c r="D35" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1286,8 +1394,11 @@
       <c r="D36" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1300,8 +1411,11 @@
       <c r="D37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1314,8 +1428,11 @@
       <c r="D38" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -1328,8 +1445,11 @@
       <c r="D39" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -1342,8 +1462,11 @@
       <c r="D40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1356,8 +1479,11 @@
       <c r="D41" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -1370,8 +1496,11 @@
       <c r="D42" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -1384,8 +1513,11 @@
       <c r="D43" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -1398,8 +1530,11 @@
       <c r="D44" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1412,8 +1547,11 @@
       <c r="D45" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1426,8 +1564,11 @@
       <c r="D46" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -1440,8 +1581,11 @@
       <c r="D47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -1454,8 +1598,11 @@
       <c r="D48" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -1468,8 +1615,11 @@
       <c r="D49" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -1482,8 +1632,11 @@
       <c r="D50" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -1496,8 +1649,11 @@
       <c r="D51" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -1510,8 +1666,11 @@
       <c r="D52" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -1524,8 +1683,11 @@
       <c r="D53" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -1538,8 +1700,11 @@
       <c r="D54" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -1552,8 +1717,11 @@
       <c r="D55" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>109</v>
       </c>
@@ -1566,8 +1734,11 @@
       <c r="D56" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -1580,8 +1751,11 @@
       <c r="D57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -1594,8 +1768,11 @@
       <c r="D58" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>112</v>
       </c>
@@ -1608,8 +1785,11 @@
       <c r="D59" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -1622,8 +1802,11 @@
       <c r="D60" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -1636,8 +1819,11 @@
       <c r="D61" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>121</v>
       </c>
@@ -1650,8 +1836,11 @@
       <c r="D62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -1664,8 +1853,11 @@
       <c r="D63" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -1678,8 +1870,11 @@
       <c r="D64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>127</v>
       </c>
@@ -1691,6 +1886,9 @@
       </c>
       <c r="D65" t="s">
         <v>125</v>
+      </c>
+      <c r="E65" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>